<commit_message>
Finished analytical portion of report
</commit_message>
<xml_diff>
--- a/Circuit Design/BOM.xlsx
+++ b/Circuit Design/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zelli\Documents\Personal Projects\TRIAC Dimmer\Circuit Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zelli\Documents\Personal Projects\Engineering\TRIAC-Dimmer\Circuit Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32DD285-82B9-4E57-A4ED-5207E4012E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BFB47D-8344-4BE8-9874-EF44B816ABAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -472,7 +472,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
PCB libraries were global, made them local
</commit_message>
<xml_diff>
--- a/Circuit Design/BOM.xlsx
+++ b/Circuit Design/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zelli\Documents\Personal Projects\Engineering\TRIAC-Dimmer\Circuit Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zelli\Documents\Personal Projects\Electronics\TRIAC-Dimmer\Circuit Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BFB47D-8344-4BE8-9874-EF44B816ABAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3B7EE6-49A6-4A1D-AF0A-E852072078D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>R1</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>CN1, CN2</t>
-  </si>
-  <si>
-    <t>sup.</t>
   </si>
   <si>
     <t>B32672L6104K000</t>
@@ -116,22 +113,22 @@
     <t>3.5A</t>
   </si>
   <si>
-    <t>F2691-ND</t>
-  </si>
-  <si>
-    <t>F1504-ND</t>
-  </si>
-  <si>
     <t>TP1, TP2, TP3</t>
   </si>
   <si>
-    <t>36-5271-ND</t>
-  </si>
-  <si>
     <t>BTB04-600SL</t>
   </si>
   <si>
-    <t>Need Model</t>
+    <t>man. pn.</t>
+  </si>
+  <si>
+    <t>023403.5MXP</t>
+  </si>
+  <si>
+    <t>05200101Z</t>
+  </si>
+  <si>
+    <t>F1 Holder</t>
   </si>
 </sst>
 </file>
@@ -469,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,73 +477,70 @@
     <col min="3" max="3" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -554,7 +548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -562,7 +556,7 @@
         <v>1726480102</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -570,28 +564,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>26</v>
+      <c r="C12" s="2">
+        <v>5271</v>
       </c>
     </row>
   </sheetData>
@@ -606,7 +603,7 @@
     <hyperlink ref="C3" r:id="rId8" xr:uid="{E262704B-C6D9-482A-824D-FA06FBBEEDB6}"/>
     <hyperlink ref="C10" r:id="rId9" xr:uid="{A33B7C8C-73EE-42EC-9C84-02B0421820D9}"/>
     <hyperlink ref="C11" r:id="rId10" xr:uid="{02AFD6D7-99D9-4449-8211-54521B9FE258}"/>
-    <hyperlink ref="C12" r:id="rId11" xr:uid="{4A4D63E6-48F6-4FDC-BDAB-39C412D13F06}"/>
+    <hyperlink ref="C12" r:id="rId11" display="5271" xr:uid="{4A4D63E6-48F6-4FDC-BDAB-39C412D13F06}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>